<commit_message>
creación modelo test para pagos, cambios menores en frontend
</commit_message>
<xml_diff>
--- a/src/FichasClientes.xlsx
+++ b/src/FichasClientes.xlsx
@@ -30,7 +30,7 @@
       <b val="1"/>
       <strike val="0"/>
       <color rgb="00808080"/>
-      <sz val="20"/>
+      <sz val="18"/>
     </font>
     <font>
       <name val="Century Gothic"/>
@@ -40,15 +40,20 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DCE6F1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -56,16 +61,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <right style="thin">
+        <color rgb="00808080"/>
+      </right>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00808080"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="00808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="00808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00808080"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="justify" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="justify" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -431,238 +482,277 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.2" customWidth="1" min="1" max="1"/>
-    <col width="21.6" customWidth="1" min="2" max="2"/>
-    <col width="21.6" customWidth="1" min="3" max="3"/>
-    <col width="15.6" customWidth="1" min="4" max="4"/>
-    <col width="20.4" customWidth="1" min="5" max="5"/>
-    <col width="16.8" customWidth="1" min="6" max="6"/>
-    <col width="24" customWidth="1" min="7" max="7"/>
-    <col width="21.6" customWidth="1" min="8" max="8"/>
-    <col width="49.2" customWidth="1" min="9" max="9"/>
-    <col width="39.6" customWidth="1" min="10" max="10"/>
-    <col width="18" customWidth="1" min="11" max="11"/>
-    <col width="32.4" customWidth="1" min="12" max="12"/>
-    <col width="21.6" customWidth="1" min="13" max="13"/>
-    <col width="25.2" customWidth="1" min="14" max="14"/>
-    <col width="27.6" customWidth="1" min="15" max="15"/>
-    <col width="24" customWidth="1" min="16" max="16"/>
-    <col width="12" customWidth="1" min="17" max="17"/>
-    <col width="9.6" customWidth="1" min="18" max="18"/>
-    <col width="20.4" customWidth="1" min="19" max="19"/>
+    <col width="27" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="79" customWidth="1" min="9" max="9"/>
+    <col width="166" customWidth="1" min="10" max="10"/>
+    <col width="15" customWidth="1" min="11" max="11"/>
+    <col width="19" customWidth="1" min="12" max="12"/>
+    <col width="22" customWidth="1" min="13" max="13"/>
+    <col width="18" customWidth="1" min="14" max="14"/>
+    <col width="21" customWidth="1" min="15" max="15"/>
+    <col width="7" customWidth="1" min="16" max="16"/>
+    <col width="23" customWidth="1" min="17" max="17"/>
+    <col width="20" customWidth="1" min="18" max="18"/>
+    <col width="10" customWidth="1" min="19" max="19"/>
+    <col width="8" customWidth="1" min="20" max="20"/>
+    <col width="17" customWidth="1" min="21" max="21"/>
   </cols>
   <sheetData>
     <row r="1" ht="24" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>CLIENTES</t>
+          <t>Datos Representante Legal</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>Datos Empresa</t>
+        </is>
+      </c>
+      <c r="L1" s="3" t="inlineStr">
+        <is>
+          <t>Datos Financieros</t>
+        </is>
+      </c>
+      <c r="P1" s="4" t="n"/>
+      <c r="Q1" s="5" t="inlineStr">
+        <is>
+          <t>Datos de Contacto</t>
+        </is>
+      </c>
+      <c r="U1" s="3" t="inlineStr">
+        <is>
+          <t>Otros</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="6" t="inlineStr">
         <is>
           <t>Nombre(s)</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="6" t="inlineStr">
         <is>
           <t>Apellido Paterno</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>Apellido Materno</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D2" s="6" t="inlineStr">
         <is>
           <t>RUN</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="E2" s="7" t="inlineStr">
         <is>
           <t>Tipo de Empresa</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="F2" s="6" t="inlineStr">
         <is>
           <t>Razón Social</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
+      <c r="G2" s="6" t="inlineStr">
         <is>
           <t>Nombre de fantasía</t>
         </is>
       </c>
-      <c r="H2" s="2" t="inlineStr">
+      <c r="H2" s="6" t="inlineStr">
         <is>
           <t>RUN</t>
         </is>
       </c>
-      <c r="I2" s="2" t="inlineStr">
+      <c r="I2" s="6" t="inlineStr">
         <is>
           <t>Régimen Tributario</t>
         </is>
       </c>
-      <c r="J2" s="2" t="inlineStr">
+      <c r="J2" s="6" t="inlineStr">
         <is>
           <t>Giro / Rubro</t>
         </is>
       </c>
-      <c r="K2" s="2" t="inlineStr">
+      <c r="K2" s="6" t="inlineStr">
         <is>
           <t>Código S.I.I.</t>
         </is>
       </c>
-      <c r="L2" s="2" t="inlineStr">
+      <c r="L2" s="6" t="inlineStr">
+        <is>
+          <t>Trabajadores</t>
+        </is>
+      </c>
+      <c r="M2" s="6" t="inlineStr">
         <is>
           <t>Tipo de contabilidad</t>
         </is>
       </c>
-      <c r="M2" s="2" t="inlineStr">
+      <c r="N2" s="6" t="inlineStr">
         <is>
           <t>Cuenta corriente</t>
         </is>
       </c>
-      <c r="N2" s="2" t="inlineStr">
+      <c r="O2" s="6" t="inlineStr">
         <is>
           <t>N° Cuenta Corriente</t>
         </is>
       </c>
-      <c r="O2" s="2" t="inlineStr">
+      <c r="P2" s="6" t="inlineStr">
+        <is>
+          <t>Deuda</t>
+        </is>
+      </c>
+      <c r="Q2" s="6" t="inlineStr">
         <is>
           <t>Correo electrónico</t>
         </is>
       </c>
-      <c r="P2" s="2" t="inlineStr">
+      <c r="R2" s="6" t="inlineStr">
         <is>
           <t>Teléfono / Celular</t>
         </is>
       </c>
-      <c r="Q2" s="2" t="inlineStr">
+      <c r="S2" s="6" t="inlineStr">
         <is>
           <t>Región</t>
         </is>
       </c>
-      <c r="R2" s="2" t="inlineStr">
+      <c r="T2" s="6" t="inlineStr">
         <is>
           <t>Comuna</t>
         </is>
       </c>
-      <c r="S2" s="2" t="inlineStr">
+      <c r="U2" s="6" t="inlineStr">
         <is>
           <t>Dirección</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="8" t="inlineStr">
         <is>
           <t>Segundo</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="8" t="inlineStr">
         <is>
           <t>Apellidos</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="8" t="inlineStr">
         <is>
           <t>Apellidotres</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="8" t="inlineStr">
+        <is>
+          <t>12345678-9</t>
+        </is>
+      </c>
+      <c r="E3" s="8" t="inlineStr">
+        <is>
+          <t>Persona Jurídica</t>
+        </is>
+      </c>
+      <c r="F3" s="8" t="inlineStr">
         <is>
           <t>razn Social</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="G3" s="8" t="inlineStr">
         <is>
           <t>nuaj</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="H3" s="8" t="inlineStr">
         <is>
           <t>12345678-9</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>12345678-9</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Persona Jurídica</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Régimen Pro PyME Transparente (14D N°8)</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Explotación De Minas Y Canteras</t>
-        </is>
-      </c>
-      <c r="K3" t="n">
-        <v>11500</v>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>Contabilidad Simplificada</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
+      <c r="I3" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Régimen Pro PyME Transparente (14D N°8)
+Régimen Para Pequeños Contribuyentes
+</t>
+        </is>
+      </c>
+      <c r="J3" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Suministro De Electricidad, Gas, Vapor Y Aire Acondicionado
+Suministro De Agua; Evacuación De Aguas Residuales, Gestión De Desechos Y Descontaminación
+Construcción
+</t>
+        </is>
+      </c>
+      <c r="K3" s="8" t="inlineStr"/>
+      <c r="L3" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="M3" s="8" t="inlineStr"/>
+      <c r="N3" s="8" t="inlineStr">
         <is>
           <t>Banco Ripley</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="O3" s="8" t="inlineStr">
         <is>
           <t>2222222222</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="Q3" s="8" t="inlineStr">
         <is>
           <t>correo@electronico.cl</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="R3" s="8" t="inlineStr">
         <is>
           <t>+5691234567</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="S3" s="8" t="inlineStr">
         <is>
           <t>Tarapacá</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="T3" s="8" t="inlineStr">
         <is>
           <t>Pica</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="U3" s="8" t="inlineStr">
         <is>
           <t>calle real #123</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:S1"/>
+  <mergeCells count="4">
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="L1:P1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>